<commit_message>
Add punctuation issues in temporal reference
</commit_message>
<xml_diff>
--- a/input_data/data_errors/3_cenarios_e_referencia_temporal/referencia_temporal.xlsx
+++ b/input_data/data_errors/3_cenarios_e_referencia_temporal/referencia_temporal.xlsx
@@ -25,13 +25,13 @@
     <t>simbolo</t>
   </si>
   <si>
-    <t>Tempo Presente</t>
+    <t>Tempo Presente.</t>
   </si>
   <si>
     <t>Déccadda de 2030</t>
   </si>
   <si>
-    <t>Década de 2050</t>
+    <t>Década de 2050.</t>
   </si>
 </sst>
 </file>

</xml_diff>